<commit_message>
Update project files and configurations
</commit_message>
<xml_diff>
--- a/data/raw/구분상가매매.xlsx
+++ b/data/raw/구분상가매매.xlsx
@@ -2348,7 +2348,7 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2706,7 +2706,7 @@
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2898,7 +2898,7 @@
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2998,7 +2998,7 @@
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -4066,7 +4066,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -4748,12 +4748,12 @@
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>4.90%</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
@@ -5044,7 +5044,7 @@
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -5927,7 +5927,7 @@
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>4.90%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="Q58" t="inlineStr"/>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>4.90%</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr">
@@ -6206,7 +6206,7 @@
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -6576,7 +6576,7 @@
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -7072,7 +7072,7 @@
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -7180,7 +7180,7 @@
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -7371,7 +7371,7 @@
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -7479,7 +7479,7 @@
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -7777,7 +7777,7 @@
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -7890,7 +7890,7 @@
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>4.90%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="Q78" t="inlineStr">
@@ -8163,7 +8163,7 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -9039,7 +9039,7 @@
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
@@ -9751,7 +9751,7 @@
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P97" t="inlineStr">
@@ -9959,7 +9959,7 @@
       <c r="N99" t="inlineStr"/>
       <c r="O99" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P99" t="inlineStr">
@@ -10153,7 +10153,7 @@
       </c>
       <c r="O101" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P101" t="inlineStr">
@@ -10239,7 +10239,7 @@
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P102" t="inlineStr">
@@ -10331,7 +10331,7 @@
       <c r="N103" t="inlineStr"/>
       <c r="O103" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P103" t="inlineStr">
@@ -10513,7 +10513,7 @@
       </c>
       <c r="O105" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P105" t="inlineStr">
@@ -11543,7 +11543,7 @@
       <c r="N117" t="inlineStr"/>
       <c r="O117" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P117" t="inlineStr">
@@ -11631,7 +11631,7 @@
       <c r="N118" t="inlineStr"/>
       <c r="O118" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P118" t="inlineStr">
@@ -11903,7 +11903,7 @@
       <c r="N121" t="inlineStr"/>
       <c r="O121" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P121" t="inlineStr">
@@ -12251,7 +12251,7 @@
       <c r="N125" t="inlineStr"/>
       <c r="O125" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P125" t="inlineStr">
@@ -12351,7 +12351,7 @@
       </c>
       <c r="O126" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P126" t="inlineStr">
@@ -12625,7 +12625,7 @@
       <c r="N129" t="inlineStr"/>
       <c r="O129" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P129" t="inlineStr">
@@ -12911,7 +12911,7 @@
       <c r="N132" t="inlineStr"/>
       <c r="O132" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P132" t="inlineStr">
@@ -13011,7 +13011,7 @@
       <c r="N133" t="inlineStr"/>
       <c r="O133" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P133" t="inlineStr">
@@ -13591,7 +13591,7 @@
       <c r="N139" t="inlineStr"/>
       <c r="O139" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P139" t="inlineStr">
@@ -14244,7 +14244,7 @@
       </c>
       <c r="O146" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P146" t="inlineStr">
@@ -14604,7 +14604,7 @@
       <c r="N150" t="inlineStr"/>
       <c r="O150" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P150" t="inlineStr">
@@ -14906,7 +14906,7 @@
       </c>
       <c r="O153" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P153" t="inlineStr">
@@ -15006,7 +15006,7 @@
       </c>
       <c r="O154" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P154" t="inlineStr">
@@ -15210,7 +15210,7 @@
       </c>
       <c r="O156" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P156" t="inlineStr">
@@ -15831,7 +15831,7 @@
       </c>
       <c r="P162" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>4.90%</t>
         </is>
       </c>
       <c r="Q162" t="inlineStr">
@@ -15926,7 +15926,7 @@
       </c>
       <c r="O163" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P163" t="inlineStr">
@@ -16030,7 +16030,7 @@
       </c>
       <c r="O164" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P164" t="inlineStr">
@@ -16395,7 +16395,7 @@
       </c>
       <c r="O168" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P168" t="inlineStr">
@@ -16483,7 +16483,7 @@
       </c>
       <c r="O169" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P169" t="inlineStr">
@@ -16571,7 +16571,7 @@
       </c>
       <c r="O170" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P170" t="inlineStr">
@@ -16819,7 +16819,7 @@
       <c r="N173" t="inlineStr"/>
       <c r="O173" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P173" t="inlineStr">
@@ -16919,7 +16919,7 @@
       </c>
       <c r="O174" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P174" t="inlineStr">
@@ -17738,7 +17738,7 @@
       </c>
       <c r="N182" t="inlineStr">
         <is>
-          <t>1400</t>
+          <t>1400.00</t>
         </is>
       </c>
       <c r="O182" t="inlineStr">
@@ -18052,7 +18052,7 @@
       </c>
       <c r="O185" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P185" t="inlineStr">
@@ -18369,7 +18369,7 @@
       <c r="N188" t="inlineStr"/>
       <c r="O188" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P188" t="inlineStr">
@@ -18654,7 +18654,7 @@
       <c r="N191" t="inlineStr"/>
       <c r="O191" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P191" t="inlineStr">
@@ -19654,7 +19654,7 @@
       <c r="N202" t="inlineStr"/>
       <c r="O202" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P202" t="inlineStr">
@@ -19754,7 +19754,7 @@
       </c>
       <c r="O203" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P203" t="inlineStr">
@@ -19888,7 +19888,7 @@
       <c r="N205" t="inlineStr"/>
       <c r="O205" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P205" t="inlineStr">
@@ -19986,7 +19986,7 @@
       </c>
       <c r="O206" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P206" t="inlineStr">
@@ -20264,7 +20264,7 @@
       <c r="N209" t="inlineStr"/>
       <c r="O209" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P209" t="inlineStr">
@@ -21112,7 +21112,7 @@
       </c>
       <c r="O218" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P218" t="inlineStr">
@@ -21216,7 +21216,7 @@
       <c r="N219" t="inlineStr"/>
       <c r="O219" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P219" t="inlineStr">
@@ -21500,7 +21500,7 @@
       <c r="N222" t="inlineStr"/>
       <c r="O222" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P222" t="inlineStr">
@@ -21561,7 +21561,7 @@
       </c>
       <c r="P223" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>4.50%</t>
         </is>
       </c>
       <c r="Q223" t="inlineStr"/>
@@ -67386,7 +67386,7 @@
       <c r="N2128" t="inlineStr"/>
       <c r="O2128" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P2128" t="inlineStr">
@@ -67514,7 +67514,7 @@
       <c r="N2132" t="inlineStr"/>
       <c r="O2132" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P2132" t="inlineStr">
@@ -67546,7 +67546,7 @@
       <c r="N2133" t="inlineStr"/>
       <c r="O2133" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P2133" t="inlineStr">
@@ -67583,7 +67583,7 @@
       </c>
       <c r="P2134" t="inlineStr">
         <is>
-          <t>3.50%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="Q2134" t="inlineStr"/>
@@ -67674,7 +67674,7 @@
       <c r="N2137" t="inlineStr"/>
       <c r="O2137" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P2137" t="inlineStr">
@@ -67710,7 +67710,7 @@
       <c r="N2138" t="inlineStr"/>
       <c r="O2138" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P2138" t="inlineStr">

</xml_diff>

<commit_message>
Fix listing add service: correct row number calculation and VLOOKUP function generation
</commit_message>
<xml_diff>
--- a/data/raw/구분상가매매.xlsx
+++ b/data/raw/구분상가매매.xlsx
@@ -2452,7 +2452,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2624,7 +2624,7 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -3202,7 +3202,7 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3974,7 +3974,7 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -4066,7 +4066,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -4166,7 +4166,7 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>4.88%</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr"/>
@@ -4648,7 +4648,7 @@
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4844,7 +4844,7 @@
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -5328,7 +5328,7 @@
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -5848,7 +5848,7 @@
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -6760,7 +6760,7 @@
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -7479,7 +7479,7 @@
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -8643,7 +8643,7 @@
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -8935,7 +8935,7 @@
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
@@ -9352,7 +9352,7 @@
       </c>
       <c r="P93" t="inlineStr">
         <is>
-          <t>4.90%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="Q93" t="inlineStr">
@@ -9547,7 +9547,7 @@
       </c>
       <c r="O95" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P95" t="inlineStr">
@@ -9647,7 +9647,7 @@
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P96" t="inlineStr">
@@ -10064,7 +10064,7 @@
       </c>
       <c r="P100" t="inlineStr">
         <is>
-          <t>4.90%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="Q100" t="inlineStr">
@@ -10431,7 +10431,7 @@
       </c>
       <c r="O104" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P104" t="inlineStr">
@@ -10605,7 +10605,7 @@
       </c>
       <c r="O106" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P106" t="inlineStr">
@@ -10973,7 +10973,7 @@
       </c>
       <c r="O110" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P110" t="inlineStr">
@@ -11059,7 +11059,7 @@
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P111" t="inlineStr">
@@ -11145,7 +11145,7 @@
       </c>
       <c r="O112" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P112" t="inlineStr">
@@ -11447,7 +11447,7 @@
       </c>
       <c r="O116" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P116" t="inlineStr">
@@ -11631,7 +11631,7 @@
       <c r="N118" t="inlineStr"/>
       <c r="O118" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P118" t="inlineStr">
@@ -11811,7 +11811,7 @@
       <c r="N120" t="inlineStr"/>
       <c r="O120" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P120" t="inlineStr">
@@ -12351,7 +12351,7 @@
       </c>
       <c r="O126" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P126" t="inlineStr">
@@ -12541,7 +12541,7 @@
       </c>
       <c r="O128" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P128" t="inlineStr">
@@ -12625,7 +12625,7 @@
       <c r="N129" t="inlineStr"/>
       <c r="O129" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P129" t="inlineStr">
@@ -12815,7 +12815,7 @@
       </c>
       <c r="O131" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P131" t="inlineStr">
@@ -12911,7 +12911,7 @@
       <c r="N132" t="inlineStr"/>
       <c r="O132" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P132" t="inlineStr">
@@ -13119,7 +13119,7 @@
       </c>
       <c r="O134" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P134" t="inlineStr">
@@ -13509,7 +13509,7 @@
       <c r="N138" t="inlineStr"/>
       <c r="O138" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P138" t="inlineStr">
@@ -14056,7 +14056,7 @@
       <c r="N144" t="inlineStr"/>
       <c r="O144" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P144" t="inlineStr">
@@ -14148,7 +14148,7 @@
       </c>
       <c r="O145" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P145" t="inlineStr">
@@ -14436,7 +14436,7 @@
       </c>
       <c r="O148" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P148" t="inlineStr">
@@ -15006,7 +15006,7 @@
       </c>
       <c r="O154" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P154" t="inlineStr">
@@ -15726,7 +15726,7 @@
       </c>
       <c r="O161" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P161" t="inlineStr">
@@ -16219,7 +16219,7 @@
       </c>
       <c r="O166" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P166" t="inlineStr">
@@ -16303,7 +16303,7 @@
       <c r="N167" t="inlineStr"/>
       <c r="O167" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P167" t="inlineStr">
@@ -17023,7 +17023,7 @@
       </c>
       <c r="O175" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P175" t="inlineStr">
@@ -17231,7 +17231,7 @@
       </c>
       <c r="O177" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P177" t="inlineStr">
@@ -17335,7 +17335,7 @@
       </c>
       <c r="O178" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P178" t="inlineStr">
@@ -18052,7 +18052,7 @@
       </c>
       <c r="O185" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P185" t="inlineStr">
@@ -19046,7 +19046,7 @@
       </c>
       <c r="O195" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P195" t="inlineStr">
@@ -19382,7 +19382,7 @@
       <c r="N199" t="inlineStr"/>
       <c r="O199" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P199" t="inlineStr">
@@ -19566,7 +19566,7 @@
       <c r="N201" t="inlineStr"/>
       <c r="O201" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P201" t="inlineStr">
@@ -19654,7 +19654,7 @@
       <c r="N202" t="inlineStr"/>
       <c r="O202" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P202" t="inlineStr">
@@ -19812,7 +19812,7 @@
       </c>
       <c r="O204" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P204" t="inlineStr">
@@ -20720,7 +20720,7 @@
       <c r="N214" t="inlineStr"/>
       <c r="O214" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P214" t="inlineStr">
@@ -21841,7 +21841,7 @@
       <c r="N226" t="inlineStr"/>
       <c r="O226" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P226" t="inlineStr">
@@ -21917,7 +21917,7 @@
       <c r="N227" t="inlineStr"/>
       <c r="O227" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P227" t="inlineStr">
@@ -22085,7 +22085,7 @@
       <c r="N229" t="inlineStr"/>
       <c r="O229" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P229" t="inlineStr">
@@ -22213,7 +22213,7 @@
       <c r="N231" t="inlineStr"/>
       <c r="O231" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P231" t="inlineStr">
@@ -67915,7 +67915,7 @@
       <c r="N2130" t="inlineStr"/>
       <c r="O2130" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P2130" t="inlineStr">
@@ -67947,7 +67947,7 @@
       <c r="N2131" t="inlineStr"/>
       <c r="O2131" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P2131" t="inlineStr">
@@ -68075,7 +68075,7 @@
       <c r="N2135" t="inlineStr"/>
       <c r="O2135" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P2135" t="inlineStr">

</xml_diff>

<commit_message>
fix: saveManagerName 함수에서 null 체크 추가
</commit_message>
<xml_diff>
--- a/data/raw/구분상가매매.xlsx
+++ b/data/raw/구분상가매매.xlsx
@@ -2348,7 +2348,7 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -3202,7 +3202,7 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3584,7 +3584,7 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -4648,7 +4648,7 @@
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4944,7 +4944,7 @@
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -5044,7 +5044,7 @@
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -5541,7 +5541,7 @@
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>4.90%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="Q54" t="inlineStr">
@@ -5752,7 +5752,7 @@
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -5848,7 +5848,7 @@
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -6116,7 +6116,7 @@
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -6206,7 +6206,7 @@
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -6576,7 +6576,7 @@
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -6760,7 +6760,7 @@
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -7072,7 +7072,7 @@
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -7180,7 +7180,7 @@
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -7371,7 +7371,7 @@
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -7885,7 +7885,7 @@
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -8069,7 +8069,7 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -8163,7 +8163,7 @@
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -8259,7 +8259,7 @@
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -8643,7 +8643,7 @@
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -9039,7 +9039,7 @@
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
@@ -9252,7 +9252,7 @@
       </c>
       <c r="P92" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>4.90%</t>
         </is>
       </c>
       <c r="Q92" t="inlineStr">
@@ -9647,7 +9647,7 @@
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P96" t="inlineStr">
@@ -9751,7 +9751,7 @@
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P97" t="inlineStr">
@@ -10239,7 +10239,7 @@
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P102" t="inlineStr">
@@ -10513,7 +10513,7 @@
       </c>
       <c r="O105" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P105" t="inlineStr">
@@ -10605,7 +10605,7 @@
       </c>
       <c r="O106" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P106" t="inlineStr">
@@ -11719,7 +11719,7 @@
       <c r="N119" t="inlineStr"/>
       <c r="O119" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P119" t="inlineStr">
@@ -12055,7 +12055,7 @@
       <c r="N123" t="inlineStr"/>
       <c r="O123" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P123" t="inlineStr">
@@ -12351,7 +12351,7 @@
       </c>
       <c r="O126" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P126" t="inlineStr">
@@ -12447,7 +12447,7 @@
       </c>
       <c r="O127" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P127" t="inlineStr">
@@ -12541,7 +12541,7 @@
       </c>
       <c r="O128" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P128" t="inlineStr">
@@ -12711,7 +12711,7 @@
       </c>
       <c r="O130" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P130" t="inlineStr">
@@ -13215,7 +13215,7 @@
       <c r="N135" t="inlineStr"/>
       <c r="O135" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P135" t="inlineStr">
@@ -13416,7 +13416,7 @@
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P137" t="inlineStr">
@@ -13509,7 +13509,7 @@
       <c r="N138" t="inlineStr"/>
       <c r="O138" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P138" t="inlineStr">
@@ -13880,7 +13880,7 @@
       <c r="N142" t="inlineStr"/>
       <c r="O142" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P142" t="inlineStr">
@@ -13964,7 +13964,7 @@
       <c r="N143" t="inlineStr"/>
       <c r="O143" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P143" t="inlineStr">
@@ -14056,7 +14056,7 @@
       <c r="N144" t="inlineStr"/>
       <c r="O144" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P144" t="inlineStr">
@@ -14148,7 +14148,7 @@
       </c>
       <c r="O145" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P145" t="inlineStr">
@@ -14436,7 +14436,7 @@
       </c>
       <c r="O148" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P148" t="inlineStr">
@@ -14710,7 +14710,7 @@
       </c>
       <c r="O151" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P151" t="inlineStr">
@@ -14806,7 +14806,7 @@
       </c>
       <c r="O152" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P152" t="inlineStr">
@@ -15006,7 +15006,7 @@
       </c>
       <c r="O154" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P154" t="inlineStr">
@@ -15418,7 +15418,7 @@
       </c>
       <c r="O158" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P158" t="inlineStr">
@@ -15826,7 +15826,7 @@
       </c>
       <c r="O162" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P162" t="inlineStr">
@@ -15926,7 +15926,7 @@
       </c>
       <c r="O163" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P163" t="inlineStr">
@@ -16219,7 +16219,7 @@
       </c>
       <c r="O166" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P166" t="inlineStr">
@@ -16303,7 +16303,7 @@
       <c r="N167" t="inlineStr"/>
       <c r="O167" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P167" t="inlineStr">
@@ -16571,7 +16571,7 @@
       </c>
       <c r="O170" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P170" t="inlineStr">
@@ -17023,7 +17023,7 @@
       </c>
       <c r="O175" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P175" t="inlineStr">
@@ -17231,12 +17231,12 @@
       </c>
       <c r="O177" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P177" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>4.90%</t>
         </is>
       </c>
       <c r="Q177" t="inlineStr">
@@ -17551,7 +17551,7 @@
       </c>
       <c r="O180" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P180" t="inlineStr">
@@ -18052,7 +18052,7 @@
       </c>
       <c r="O185" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P185" t="inlineStr">
@@ -18161,7 +18161,7 @@
       </c>
       <c r="O186" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P186" t="inlineStr">
@@ -18457,7 +18457,7 @@
       <c r="N189" t="inlineStr"/>
       <c r="O189" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P189" t="inlineStr">
@@ -18566,7 +18566,7 @@
       </c>
       <c r="O190" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P190" t="inlineStr">
@@ -18654,7 +18654,7 @@
       <c r="N191" t="inlineStr"/>
       <c r="O191" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P191" t="inlineStr">
@@ -19566,7 +19566,7 @@
       <c r="N201" t="inlineStr"/>
       <c r="O201" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P201" t="inlineStr">
@@ -19986,7 +19986,7 @@
       </c>
       <c r="O206" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P206" t="inlineStr">
@@ -20081,12 +20081,12 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1000.00</t>
         </is>
       </c>
       <c r="O207" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P207" t="inlineStr">
@@ -20720,7 +20720,7 @@
       <c r="N214" t="inlineStr"/>
       <c r="O214" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P214" t="inlineStr">
@@ -21112,7 +21112,7 @@
       </c>
       <c r="O218" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P218" t="inlineStr">
@@ -21216,7 +21216,7 @@
       <c r="N219" t="inlineStr"/>
       <c r="O219" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P219" t="inlineStr">
@@ -21408,12 +21408,12 @@
       <c r="N221" t="inlineStr"/>
       <c r="O221" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P221" t="inlineStr">
         <is>
-          <t>4.90%</t>
+          <t>5%</t>
         </is>
       </c>
       <c r="Q221" t="inlineStr"/>
@@ -21500,7 +21500,7 @@
       <c r="N222" t="inlineStr"/>
       <c r="O222" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P222" t="inlineStr">
@@ -21765,7 +21765,7 @@
       <c r="N225" t="inlineStr"/>
       <c r="O225" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P225" t="inlineStr">
@@ -68011,7 +68011,7 @@
       <c r="N2134" t="inlineStr"/>
       <c r="O2134" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="P2134" t="inlineStr">
@@ -68043,7 +68043,7 @@
       <c r="N2135" t="inlineStr"/>
       <c r="O2135" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="P2135" t="inlineStr">

</xml_diff>